<commit_message>
Add NIST data base
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC57"/>
+  <dimension ref="A1:AQ57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,6 +580,76 @@
           <t>T1 - cortical GM</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 2</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 3</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 4</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 5</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 6</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 7</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 8</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 9</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 10</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 11</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 12</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 13</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 14</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -597,7 +667,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20200103_refaatgabr_mcgovern_human/20200103_refaatgabr_mcgovern_human_t1map.nii.gz</t>
+          <t>20200103_refaatgabr_mcgovern_human/20200103_refaatgabr_mcgovern_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -705,6 +775,20 @@
  2368.2 2452.7 2320.4 2600.7 2505.6 2293.5 2668. ]</t>
         </is>
       </c>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -722,7 +806,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject01_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject01_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -832,6 +916,20 @@
  1328.6 1492.5 1343.2 1297.7 1445.9 1332.3 1316.7]</t>
         </is>
       </c>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -849,7 +947,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject02_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject02_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -955,6 +1053,20 @@
  1268.1 1340.7 1536.1 1534.9 1428.6 1593.6 1522.3 1414.2]</t>
         </is>
       </c>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -972,7 +1084,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject03_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject03_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1082,6 +1194,20 @@
  1510.5 1409.9 1401.7 1500.6 1398.1 1295.9 1335.3]</t>
         </is>
       </c>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1099,7 +1225,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200206_mrel_usc_GE3T_MR1_human_subject04_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200206_mrel_usc_GE3T_MR1_human_subject04_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1210,6 +1336,20 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1227,7 +1367,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject05_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject05_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1337,6 +1477,20 @@
  1463.  1547.1 1446.6 1557.7 1687.  1431.3 1582.2]</t>
         </is>
       </c>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1354,7 +1508,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject06_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject06_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1464,6 +1618,20 @@
  1305.5 1418.7 1444.6 1464.9 1143.6 1383.8 1560.2]</t>
         </is>
       </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1481,7 +1649,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>20200203_iveslevesque_muhc_mgh_human/20200203_iveslevesque_muhc_mgh_human_t1map.nii.gz</t>
+          <t>20200203_iveslevesque_muhc_mgh_human/20200203_iveslevesque_muhc_mgh_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1592,6 +1760,20 @@
  1999.5 2221.3 2238.6 2093.2 2110.  1972.1 2196.9]</t>
         </is>
       </c>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1609,7 +1791,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>20200203_siyuanhu_casewestern_human/20200203_siyuanhu_casewestern_human_t1map.nii.gz</t>
+          <t>20200203_siyuanhu_casewestern_human/20200203_siyuanhu_casewestern_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1717,6 +1899,20 @@
  1459.4 1499.8 1515.1 1750.9 1655.8 1586.4 1441.8]</t>
         </is>
       </c>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1734,7 +1930,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_20ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_20ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1842,6 +2038,20 @@
  1218.5 1606.6 1481.8 1418.  1512.9 1505.2 1583. ]</t>
         </is>
       </c>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1859,7 +2069,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_64ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_64ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1970,6 +2180,20 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1987,7 +2211,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_20ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_20ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -2099,6 +2323,20 @@
  1526.8 1436.6 1383.4 1567.3 1873.4 1817.3 1163.2 1269.1]</t>
         </is>
       </c>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -2116,7 +2354,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_64ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_64ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -2222,6 +2460,20 @@
  1144.2 1255.1 1281.6 1298.7 1237.7 1198.8 1228.7 1224.5]</t>
         </is>
       </c>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2239,7 +2491,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>20200219_marcocastellaro_UniPD_human/20200219_marcocastellaro_UniPD_human_Complex_t1map.nii.gz</t>
+          <t>20200219_marcocastellaro_UniPD_human/20200219_marcocastellaro_UniPD_human_Complex_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2349,6 +2601,20 @@
  1364.5 1665.5 1438.9 1359.4 1679.5 1397.5 1297.3]</t>
         </is>
       </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2366,7 +2632,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>20200221_madelinecarr_lha_human/20200221_madelinecarr_lha_human_t1map.nii.gz</t>
+          <t>20200221_madelinecarr_lha_human/20200221_madelinecarr_lha_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2472,6 +2738,20 @@
  1344.2 1544.2]</t>
         </is>
       </c>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2489,7 +2769,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_magnitude_t1map.nii.gz</t>
+          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_magnitude_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2596,6 +2876,20 @@
  1113.3 1249.9 1228.1 1308.6 1218.9 1309.4 1220.6 1249.1]</t>
         </is>
       </c>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2613,7 +2907,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_Complex_t1map.nii.gz</t>
+          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_Complex_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2720,6 +3014,20 @@
  1095.8 1281.5 1186.6 1278.1 1185.7 1324.1 1227.8 1243.6]</t>
         </is>
       </c>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2737,7 +3045,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200206_190116_Ph/21527_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200206_190116_Ph/21527_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2847,6 +3155,20 @@
  1391.7 1387.9 1433.5 1428.  1414.6 1411.5 1439.1]</t>
         </is>
       </c>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2864,7 +3186,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2974,6 +3296,20 @@
  1547.9 1469.3 1431.  1418.6 1651.9 1628.8 1677.9]</t>
         </is>
       </c>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr"/>
+      <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2991,7 +3327,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3101,6 +3437,20 @@
  1557.5 1466.9 1446.6 1421.9 1607.6 1585.5 1635.1]</t>
         </is>
       </c>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -3118,7 +3468,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3228,6 +3578,20 @@
  1457.8 1493.9 1555.6 1600.6 1492.3 1653.6 1682.7]</t>
         </is>
       </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -3245,7 +3609,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3355,6 +3719,20 @@
  1460.5 1499.1 1568.8 1603.8 1544.2 1650.3 1677.6]</t>
         </is>
       </c>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -3372,7 +3750,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3482,6 +3860,20 @@
  1435.  1599.7 1631.4 1496.7 1490.7 1506.3 1539.9]</t>
         </is>
       </c>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="inlineStr"/>
+      <c r="AJ24" t="inlineStr"/>
+      <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -3499,7 +3891,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3609,6 +4001,20 @@
  1476.5 1551.  1579.1 1505.9 1458.5 1468.2 1535.3]</t>
         </is>
       </c>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="inlineStr"/>
+      <c r="AJ25" t="inlineStr"/>
+      <c r="AK25" t="inlineStr"/>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
+      <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -3626,7 +4032,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_151000_Ph/56190_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_151000_Ph/56190_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3735,6 +4141,20 @@
  1511.4 1462.2 1429.5 1446.7 1445.2 1348.9 1296.2 1384. ]</t>
         </is>
       </c>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="inlineStr"/>
+      <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3752,7 +4172,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3862,6 +4282,20 @@
  1833.5 1454.2 1577.6 1591.6 1396.6 1497.2 1486.9]</t>
         </is>
       </c>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -3879,7 +4313,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3989,6 +4423,20 @@
  1810.3 1442.7 1577.  1600.2 1382.4 1470.  1487.6]</t>
         </is>
       </c>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -4006,7 +4454,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_133135_Ph/56961_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_133135_Ph/56961_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -4112,6 +4560,20 @@
  1518.9 1444.3 1251.4 1141.8 1403.7 1232.  1563.8 1386.9]</t>
         </is>
       </c>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="inlineStr"/>
+      <c r="AK29" t="inlineStr"/>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
+      <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="inlineStr"/>
+      <c r="AQ29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -4129,7 +4591,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_141051_Ph/58416_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_141051_Ph/58416_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -4239,6 +4701,20 @@
  1678.1 1732.  1776.9 1759.3 1766.8 1758.8 1862.8]</t>
         </is>
       </c>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr"/>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
+      <c r="AO30" t="inlineStr"/>
+      <c r="AP30" t="inlineStr"/>
+      <c r="AQ30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -4256,7 +4732,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -4366,6 +4842,20 @@
  1552.5 1596.1 1644.6 1711.  1463.8 1487.3 1561.3]</t>
         </is>
       </c>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="inlineStr"/>
+      <c r="AK31" t="inlineStr"/>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
+      <c r="AO31" t="inlineStr"/>
+      <c r="AP31" t="inlineStr"/>
+      <c r="AQ31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -4383,7 +4873,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -4493,6 +4983,20 @@
  1520.9 1588.  1658.3 1740.9 1444.8 1501.9 1645.5]</t>
         </is>
       </c>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr"/>
+      <c r="AJ32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr"/>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
+      <c r="AO32" t="inlineStr"/>
+      <c r="AP32" t="inlineStr"/>
+      <c r="AQ32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -4510,7 +5014,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_145118_Ph/58139_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_145118_Ph/58139_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -4616,6 +5120,20 @@
  1686.4 1607.5 1561.4 1633.2 1703.9 1696.5 1751.7 1621.8]</t>
         </is>
       </c>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
+      <c r="AP33" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -4633,7 +5151,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -4743,6 +5261,20 @@
  1736.7 1422.4 1488.7 1722.2 1488.9 1563.1 1694.2]</t>
         </is>
       </c>
+      <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr"/>
+      <c r="AG34" t="inlineStr"/>
+      <c r="AH34" t="inlineStr"/>
+      <c r="AI34" t="inlineStr"/>
+      <c r="AJ34" t="inlineStr"/>
+      <c r="AK34" t="inlineStr"/>
+      <c r="AL34" t="inlineStr"/>
+      <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr"/>
+      <c r="AO34" t="inlineStr"/>
+      <c r="AP34" t="inlineStr"/>
+      <c r="AQ34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -4760,7 +5292,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4870,6 +5402,20 @@
  1691.1 1483.4 1526.1 1666.9 1525.3 1575.  1658.8]</t>
         </is>
       </c>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr"/>
+      <c r="AG35" t="inlineStr"/>
+      <c r="AH35" t="inlineStr"/>
+      <c r="AI35" t="inlineStr"/>
+      <c r="AJ35" t="inlineStr"/>
+      <c r="AK35" t="inlineStr"/>
+      <c r="AL35" t="inlineStr"/>
+      <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr"/>
+      <c r="AO35" t="inlineStr"/>
+      <c r="AP35" t="inlineStr"/>
+      <c r="AQ35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -4887,7 +5433,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58173/20200206_182142_Ph/58173_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58173/20200206_182142_Ph/58173_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4997,6 +5543,20 @@
  1586.2 1706.5 1903.8 1716.4 1622.5 1660.6 1766.8]</t>
         </is>
       </c>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="inlineStr"/>
+      <c r="AH36" t="inlineStr"/>
+      <c r="AI36" t="inlineStr"/>
+      <c r="AJ36" t="inlineStr"/>
+      <c r="AK36" t="inlineStr"/>
+      <c r="AL36" t="inlineStr"/>
+      <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr"/>
+      <c r="AO36" t="inlineStr"/>
+      <c r="AP36" t="inlineStr"/>
+      <c r="AQ36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -5014,7 +5574,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58174/20200206_184031_Ph/58174_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58174/20200206_184031_Ph/58174_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -5120,6 +5680,20 @@
  1763.4 1679.8 1748.5 1610.3 1446.4 2015.2 1639.9 1573.5]</t>
         </is>
       </c>
+      <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr"/>
+      <c r="AH37" t="inlineStr"/>
+      <c r="AI37" t="inlineStr"/>
+      <c r="AJ37" t="inlineStr"/>
+      <c r="AK37" t="inlineStr"/>
+      <c r="AL37" t="inlineStr"/>
+      <c r="AM37" t="inlineStr"/>
+      <c r="AN37" t="inlineStr"/>
+      <c r="AO37" t="inlineStr"/>
+      <c r="AP37" t="inlineStr"/>
+      <c r="AQ37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -5137,7 +5711,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -5247,6 +5821,20 @@
  1274.9 1399.  1272.8 1258.9 1379.6 1242.5 1221.4]</t>
         </is>
       </c>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr"/>
+      <c r="AG38" t="inlineStr"/>
+      <c r="AH38" t="inlineStr"/>
+      <c r="AI38" t="inlineStr"/>
+      <c r="AJ38" t="inlineStr"/>
+      <c r="AK38" t="inlineStr"/>
+      <c r="AL38" t="inlineStr"/>
+      <c r="AM38" t="inlineStr"/>
+      <c r="AN38" t="inlineStr"/>
+      <c r="AO38" t="inlineStr"/>
+      <c r="AP38" t="inlineStr"/>
+      <c r="AQ38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -5264,7 +5852,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5374,6 +5962,20 @@
  1300.6 1409.2 1277.4 1279.4 1361.6 1230.4 1239.2]</t>
         </is>
       </c>
+      <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr"/>
+      <c r="AH39" t="inlineStr"/>
+      <c r="AI39" t="inlineStr"/>
+      <c r="AJ39" t="inlineStr"/>
+      <c r="AK39" t="inlineStr"/>
+      <c r="AL39" t="inlineStr"/>
+      <c r="AM39" t="inlineStr"/>
+      <c r="AN39" t="inlineStr"/>
+      <c r="AO39" t="inlineStr"/>
+      <c r="AP39" t="inlineStr"/>
+      <c r="AQ39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -5391,7 +5993,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_124551_Ph/58414_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_124551_Ph/58414_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5501,6 +6103,20 @@
  1407.2 1457.9 1493.6 1411.3 1459.5 1442.8 1425.1]</t>
         </is>
       </c>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
+      <c r="AI40" t="inlineStr"/>
+      <c r="AJ40" t="inlineStr"/>
+      <c r="AK40" t="inlineStr"/>
+      <c r="AL40" t="inlineStr"/>
+      <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr"/>
+      <c r="AO40" t="inlineStr"/>
+      <c r="AP40" t="inlineStr"/>
+      <c r="AQ40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -5518,7 +6134,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -5628,6 +6244,20 @@
  1474.6 1577.4 1558.6 1510.1 1686.  1666.9 1622.6]</t>
         </is>
       </c>
+      <c r="AD41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr"/>
+      <c r="AI41" t="inlineStr"/>
+      <c r="AJ41" t="inlineStr"/>
+      <c r="AK41" t="inlineStr"/>
+      <c r="AL41" t="inlineStr"/>
+      <c r="AM41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr"/>
+      <c r="AO41" t="inlineStr"/>
+      <c r="AP41" t="inlineStr"/>
+      <c r="AQ41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -5645,7 +6275,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5755,6 +6385,20 @@
  1452.7 1583.3 1536.6 1499.6 1617.  1602.7 1578. ]</t>
         </is>
       </c>
+      <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr"/>
+      <c r="AI42" t="inlineStr"/>
+      <c r="AJ42" t="inlineStr"/>
+      <c r="AK42" t="inlineStr"/>
+      <c r="AL42" t="inlineStr"/>
+      <c r="AM42" t="inlineStr"/>
+      <c r="AN42" t="inlineStr"/>
+      <c r="AO42" t="inlineStr"/>
+      <c r="AP42" t="inlineStr"/>
+      <c r="AQ42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -5772,7 +6416,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -5882,6 +6526,20 @@
  1838.  2013.8 2122.  1784.  1677.  1781.9 1888.8]</t>
         </is>
       </c>
+      <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr"/>
+      <c r="AI43" t="inlineStr"/>
+      <c r="AJ43" t="inlineStr"/>
+      <c r="AK43" t="inlineStr"/>
+      <c r="AL43" t="inlineStr"/>
+      <c r="AM43" t="inlineStr"/>
+      <c r="AN43" t="inlineStr"/>
+      <c r="AO43" t="inlineStr"/>
+      <c r="AP43" t="inlineStr"/>
+      <c r="AQ43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -5899,7 +6557,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData-2_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData-2_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -6009,6 +6667,20 @@
  1835.9 1865.6 2013.6 1803.  1526.6 1683.7 1892.3]</t>
         </is>
       </c>
+      <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr"/>
+      <c r="AI44" t="inlineStr"/>
+      <c r="AJ44" t="inlineStr"/>
+      <c r="AK44" t="inlineStr"/>
+      <c r="AL44" t="inlineStr"/>
+      <c r="AM44" t="inlineStr"/>
+      <c r="AN44" t="inlineStr"/>
+      <c r="AO44" t="inlineStr"/>
+      <c r="AP44" t="inlineStr"/>
+      <c r="AQ44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -6026,7 +6698,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -6136,6 +6808,20 @@
  1392.9 1460.9 1382.6 1455.  1469.6 1379.2 1452. ]</t>
         </is>
       </c>
+      <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr"/>
+      <c r="AI45" t="inlineStr"/>
+      <c r="AJ45" t="inlineStr"/>
+      <c r="AK45" t="inlineStr"/>
+      <c r="AL45" t="inlineStr"/>
+      <c r="AM45" t="inlineStr"/>
+      <c r="AN45" t="inlineStr"/>
+      <c r="AO45" t="inlineStr"/>
+      <c r="AP45" t="inlineStr"/>
+      <c r="AQ45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -6153,7 +6839,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -6263,6 +6949,20 @@
  1401.5 1459.  1405.  1444.7 1466.  1402.5 1439.7]</t>
         </is>
       </c>
+      <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr"/>
+      <c r="AI46" t="inlineStr"/>
+      <c r="AJ46" t="inlineStr"/>
+      <c r="AK46" t="inlineStr"/>
+      <c r="AL46" t="inlineStr"/>
+      <c r="AM46" t="inlineStr"/>
+      <c r="AN46" t="inlineStr"/>
+      <c r="AO46" t="inlineStr"/>
+      <c r="AP46" t="inlineStr"/>
+      <c r="AQ46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -6280,7 +6980,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_152800_Ph/56347_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_152800_Ph/56347_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -6386,6 +7086,20 @@
  1705.6 1758.3 1563.3 1524.6 1712.9 1687.8 1720.  1678.4]</t>
         </is>
       </c>
+      <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr"/>
+      <c r="AI47" t="inlineStr"/>
+      <c r="AJ47" t="inlineStr"/>
+      <c r="AK47" t="inlineStr"/>
+      <c r="AL47" t="inlineStr"/>
+      <c r="AM47" t="inlineStr"/>
+      <c r="AN47" t="inlineStr"/>
+      <c r="AO47" t="inlineStr"/>
+      <c r="AP47" t="inlineStr"/>
+      <c r="AQ47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -6403,7 +7117,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_134934_Ph/58415_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_134934_Ph/58415_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -6513,6 +7227,20 @@
  1503.  1626.2 1574.2 1626.4 1544.4 1528.4 1530. ]</t>
         </is>
       </c>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
+      <c r="AI48" t="inlineStr"/>
+      <c r="AJ48" t="inlineStr"/>
+      <c r="AK48" t="inlineStr"/>
+      <c r="AL48" t="inlineStr"/>
+      <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr"/>
+      <c r="AO48" t="inlineStr"/>
+      <c r="AP48" t="inlineStr"/>
+      <c r="AQ48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -6530,7 +7258,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6640,6 +7368,20 @@
  1638.6 1542.1 1658.  1625.8 1585.3 1648.4 1511.2]</t>
         </is>
       </c>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
+      <c r="AI49" t="inlineStr"/>
+      <c r="AJ49" t="inlineStr"/>
+      <c r="AK49" t="inlineStr"/>
+      <c r="AL49" t="inlineStr"/>
+      <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr"/>
+      <c r="AO49" t="inlineStr"/>
+      <c r="AP49" t="inlineStr"/>
+      <c r="AQ49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -6657,7 +7399,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6767,6 +7509,20 @@
  1684.2 1517.5 1683.2 1646.2 1577.6 1671.7 1506.6]</t>
         </is>
       </c>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
+      <c r="AI50" t="inlineStr"/>
+      <c r="AJ50" t="inlineStr"/>
+      <c r="AK50" t="inlineStr"/>
+      <c r="AL50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr"/>
+      <c r="AO50" t="inlineStr"/>
+      <c r="AP50" t="inlineStr"/>
+      <c r="AQ50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -6784,7 +7540,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -6894,6 +7650,20 @@
  1518.  1544.2 1594.1 1614.8 1481.8 1674.6 1589.2]</t>
         </is>
       </c>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
+      <c r="AI51" t="inlineStr"/>
+      <c r="AJ51" t="inlineStr"/>
+      <c r="AK51" t="inlineStr"/>
+      <c r="AL51" t="inlineStr"/>
+      <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr"/>
+      <c r="AO51" t="inlineStr"/>
+      <c r="AP51" t="inlineStr"/>
+      <c r="AQ51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -6911,7 +7681,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -7021,6 +7791,20 @@
  1547.4 1568.3 1549.8 1611.1 1482.1 1585.8 1571.8]</t>
         </is>
       </c>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" t="inlineStr"/>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr"/>
+      <c r="AN52" t="inlineStr"/>
+      <c r="AO52" t="inlineStr"/>
+      <c r="AP52" t="inlineStr"/>
+      <c r="AQ52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -7038,7 +7822,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_122504_Ph/56348_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_122504_Ph/56348_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -7146,6 +7930,20 @@
           <t>[1895.6 1749.3 1537.6 1722.9 1646.6 1513.6 1669.3 1714.6 1763. ]</t>
         </is>
       </c>
+      <c r="AD53" t="inlineStr"/>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+      <c r="AO53" t="inlineStr"/>
+      <c r="AP53" t="inlineStr"/>
+      <c r="AQ53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -7163,7 +7961,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_142721_Ph/58132_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_142721_Ph/58132_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -7269,6 +8067,20 @@
  2027.4 2185.3 1878.8 1770.9 1804.8 1723.6 1783.6 1717.1]</t>
         </is>
       </c>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+      <c r="AO54" t="inlineStr"/>
+      <c r="AP54" t="inlineStr"/>
+      <c r="AQ54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -7286,7 +8098,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -7396,6 +8208,20 @@
  1437.8 1427.5 1364.7 1342.4 1438.3 1399.2 1408.7]</t>
         </is>
       </c>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+      <c r="AO55" t="inlineStr"/>
+      <c r="AP55" t="inlineStr"/>
+      <c r="AQ55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -7413,7 +8239,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -7523,6 +8349,20 @@
  1476.5 1435.3 1399.5 1380.9 1426.3 1400.5 1398.4]</t>
         </is>
       </c>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" t="inlineStr"/>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+      <c r="AO56" t="inlineStr"/>
+      <c r="AP56" t="inlineStr"/>
+      <c r="AQ56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -7540,7 +8380,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>20200226_iveslevesque_muhc_glen_human/20200226_muhc_glen_Human_t1map.nii.gz</t>
+          <t>20200226_iveslevesque_muhc_glen_human/20200226_muhc_glen_Human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -7648,6 +8488,20 @@
  1446.1 1293.4 1344.  1424.6 1326.  1352.5 1399.1]</t>
         </is>
       </c>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+      <c r="AO57" t="inlineStr"/>
+      <c r="AP57" t="inlineStr"/>
+      <c r="AQ57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Add NIST database template (no ROI values yet, will fill when #10 is completed and merged
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AC57"/>
+  <dimension ref="A1:AQ57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -580,6 +580,76 @@
           <t>T1 - cortical GM</t>
         </is>
       </c>
+      <c r="AD1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 1</t>
+        </is>
+      </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 2</t>
+        </is>
+      </c>
+      <c r="AF1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 3</t>
+        </is>
+      </c>
+      <c r="AG1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 4</t>
+        </is>
+      </c>
+      <c r="AH1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 5</t>
+        </is>
+      </c>
+      <c r="AI1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 6</t>
+        </is>
+      </c>
+      <c r="AJ1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 7</t>
+        </is>
+      </c>
+      <c r="AK1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 8</t>
+        </is>
+      </c>
+      <c r="AL1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 9</t>
+        </is>
+      </c>
+      <c r="AM1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 10</t>
+        </is>
+      </c>
+      <c r="AN1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 11</t>
+        </is>
+      </c>
+      <c r="AO1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 12</t>
+        </is>
+      </c>
+      <c r="AP1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 13</t>
+        </is>
+      </c>
+      <c r="AQ1" s="1" t="inlineStr">
+        <is>
+          <t>T1 - NIST sphere 14</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="n">
@@ -597,7 +667,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>20200103_refaatgabr_mcgovern_human/20200103_refaatgabr_mcgovern_human_t1map.nii.gz</t>
+          <t>20200103_refaatgabr_mcgovern_human/20200103_refaatgabr_mcgovern_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -705,6 +775,20 @@
  2368.2 2452.7 2320.4 2600.7 2505.6 2293.5 2668. ]</t>
         </is>
       </c>
+      <c r="AD2" t="inlineStr"/>
+      <c r="AE2" t="inlineStr"/>
+      <c r="AF2" t="inlineStr"/>
+      <c r="AG2" t="inlineStr"/>
+      <c r="AH2" t="inlineStr"/>
+      <c r="AI2" t="inlineStr"/>
+      <c r="AJ2" t="inlineStr"/>
+      <c r="AK2" t="inlineStr"/>
+      <c r="AL2" t="inlineStr"/>
+      <c r="AM2" t="inlineStr"/>
+      <c r="AN2" t="inlineStr"/>
+      <c r="AO2" t="inlineStr"/>
+      <c r="AP2" t="inlineStr"/>
+      <c r="AQ2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="n">
@@ -722,7 +806,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject01_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject01_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -832,6 +916,20 @@
  1328.6 1492.5 1343.2 1297.7 1445.9 1332.3 1316.7]</t>
         </is>
       </c>
+      <c r="AD3" t="inlineStr"/>
+      <c r="AE3" t="inlineStr"/>
+      <c r="AF3" t="inlineStr"/>
+      <c r="AG3" t="inlineStr"/>
+      <c r="AH3" t="inlineStr"/>
+      <c r="AI3" t="inlineStr"/>
+      <c r="AJ3" t="inlineStr"/>
+      <c r="AK3" t="inlineStr"/>
+      <c r="AL3" t="inlineStr"/>
+      <c r="AM3" t="inlineStr"/>
+      <c r="AN3" t="inlineStr"/>
+      <c r="AO3" t="inlineStr"/>
+      <c r="AP3" t="inlineStr"/>
+      <c r="AQ3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="n">
@@ -849,7 +947,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject02_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject02_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -955,6 +1053,20 @@
  1268.1 1340.7 1536.1 1534.9 1428.6 1593.6 1522.3 1414.2]</t>
         </is>
       </c>
+      <c r="AD4" t="inlineStr"/>
+      <c r="AE4" t="inlineStr"/>
+      <c r="AF4" t="inlineStr"/>
+      <c r="AG4" t="inlineStr"/>
+      <c r="AH4" t="inlineStr"/>
+      <c r="AI4" t="inlineStr"/>
+      <c r="AJ4" t="inlineStr"/>
+      <c r="AK4" t="inlineStr"/>
+      <c r="AL4" t="inlineStr"/>
+      <c r="AM4" t="inlineStr"/>
+      <c r="AN4" t="inlineStr"/>
+      <c r="AO4" t="inlineStr"/>
+      <c r="AP4" t="inlineStr"/>
+      <c r="AQ4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="n">
@@ -972,7 +1084,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject03_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200128_mrel_usc_GE3T_MR1_human_subject03_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -1082,6 +1194,20 @@
  1510.5 1409.9 1401.7 1500.6 1398.1 1295.9 1335.3]</t>
         </is>
       </c>
+      <c r="AD5" t="inlineStr"/>
+      <c r="AE5" t="inlineStr"/>
+      <c r="AF5" t="inlineStr"/>
+      <c r="AG5" t="inlineStr"/>
+      <c r="AH5" t="inlineStr"/>
+      <c r="AI5" t="inlineStr"/>
+      <c r="AJ5" t="inlineStr"/>
+      <c r="AK5" t="inlineStr"/>
+      <c r="AL5" t="inlineStr"/>
+      <c r="AM5" t="inlineStr"/>
+      <c r="AN5" t="inlineStr"/>
+      <c r="AO5" t="inlineStr"/>
+      <c r="AP5" t="inlineStr"/>
+      <c r="AQ5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n">
@@ -1099,7 +1225,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200206_mrel_usc_GE3T_MR1_human_subject04_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200206_mrel_usc_GE3T_MR1_human_subject04_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -1210,6 +1336,20 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="AD6" t="inlineStr"/>
+      <c r="AE6" t="inlineStr"/>
+      <c r="AF6" t="inlineStr"/>
+      <c r="AG6" t="inlineStr"/>
+      <c r="AH6" t="inlineStr"/>
+      <c r="AI6" t="inlineStr"/>
+      <c r="AJ6" t="inlineStr"/>
+      <c r="AK6" t="inlineStr"/>
+      <c r="AL6" t="inlineStr"/>
+      <c r="AM6" t="inlineStr"/>
+      <c r="AN6" t="inlineStr"/>
+      <c r="AO6" t="inlineStr"/>
+      <c r="AP6" t="inlineStr"/>
+      <c r="AQ6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="n">
@@ -1227,7 +1367,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject05_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject05_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -1337,6 +1477,20 @@
  1463.  1547.1 1446.6 1557.7 1687.  1431.3 1582.2]</t>
         </is>
       </c>
+      <c r="AD7" t="inlineStr"/>
+      <c r="AE7" t="inlineStr"/>
+      <c r="AF7" t="inlineStr"/>
+      <c r="AG7" t="inlineStr"/>
+      <c r="AH7" t="inlineStr"/>
+      <c r="AI7" t="inlineStr"/>
+      <c r="AJ7" t="inlineStr"/>
+      <c r="AK7" t="inlineStr"/>
+      <c r="AL7" t="inlineStr"/>
+      <c r="AM7" t="inlineStr"/>
+      <c r="AN7" t="inlineStr"/>
+      <c r="AO7" t="inlineStr"/>
+      <c r="AP7" t="inlineStr"/>
+      <c r="AQ7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" s="1" t="n">
@@ -1354,7 +1508,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject06_t1map.nii.gz</t>
+          <t>20200128_mrel_usc_human/20200228_mrel_usc_GE3T_MR2_human_subject06_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -1464,6 +1618,20 @@
  1305.5 1418.7 1444.6 1464.9 1143.6 1383.8 1560.2]</t>
         </is>
       </c>
+      <c r="AD8" t="inlineStr"/>
+      <c r="AE8" t="inlineStr"/>
+      <c r="AF8" t="inlineStr"/>
+      <c r="AG8" t="inlineStr"/>
+      <c r="AH8" t="inlineStr"/>
+      <c r="AI8" t="inlineStr"/>
+      <c r="AJ8" t="inlineStr"/>
+      <c r="AK8" t="inlineStr"/>
+      <c r="AL8" t="inlineStr"/>
+      <c r="AM8" t="inlineStr"/>
+      <c r="AN8" t="inlineStr"/>
+      <c r="AO8" t="inlineStr"/>
+      <c r="AP8" t="inlineStr"/>
+      <c r="AQ8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n">
@@ -1481,7 +1649,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>20200203_iveslevesque_muhc_mgh_human/20200203_iveslevesque_muhc_mgh_human_t1map.nii.gz</t>
+          <t>20200203_iveslevesque_muhc_mgh_human/20200203_iveslevesque_muhc_mgh_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -1592,6 +1760,20 @@
  1999.5 2221.3 2238.6 2093.2 2110.  1972.1 2196.9]</t>
         </is>
       </c>
+      <c r="AD9" t="inlineStr"/>
+      <c r="AE9" t="inlineStr"/>
+      <c r="AF9" t="inlineStr"/>
+      <c r="AG9" t="inlineStr"/>
+      <c r="AH9" t="inlineStr"/>
+      <c r="AI9" t="inlineStr"/>
+      <c r="AJ9" t="inlineStr"/>
+      <c r="AK9" t="inlineStr"/>
+      <c r="AL9" t="inlineStr"/>
+      <c r="AM9" t="inlineStr"/>
+      <c r="AN9" t="inlineStr"/>
+      <c r="AO9" t="inlineStr"/>
+      <c r="AP9" t="inlineStr"/>
+      <c r="AQ9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" s="1" t="n">
@@ -1609,7 +1791,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>20200203_siyuanhu_casewestern_human/20200203_siyuanhu_casewestern_human_t1map.nii.gz</t>
+          <t>20200203_siyuanhu_casewestern_human/20200203_siyuanhu_casewestern_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1717,6 +1899,20 @@
  1459.4 1499.8 1515.1 1750.9 1655.8 1586.4 1441.8]</t>
         </is>
       </c>
+      <c r="AD10" t="inlineStr"/>
+      <c r="AE10" t="inlineStr"/>
+      <c r="AF10" t="inlineStr"/>
+      <c r="AG10" t="inlineStr"/>
+      <c r="AH10" t="inlineStr"/>
+      <c r="AI10" t="inlineStr"/>
+      <c r="AJ10" t="inlineStr"/>
+      <c r="AK10" t="inlineStr"/>
+      <c r="AL10" t="inlineStr"/>
+      <c r="AM10" t="inlineStr"/>
+      <c r="AN10" t="inlineStr"/>
+      <c r="AO10" t="inlineStr"/>
+      <c r="AP10" t="inlineStr"/>
+      <c r="AQ10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" s="1" t="n">
@@ -1734,7 +1930,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_20ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_20ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -1842,6 +2038,20 @@
  1218.5 1606.6 1481.8 1418.  1512.9 1505.2 1583. ]</t>
         </is>
       </c>
+      <c r="AD11" t="inlineStr"/>
+      <c r="AE11" t="inlineStr"/>
+      <c r="AF11" t="inlineStr"/>
+      <c r="AG11" t="inlineStr"/>
+      <c r="AH11" t="inlineStr"/>
+      <c r="AI11" t="inlineStr"/>
+      <c r="AJ11" t="inlineStr"/>
+      <c r="AK11" t="inlineStr"/>
+      <c r="AL11" t="inlineStr"/>
+      <c r="AM11" t="inlineStr"/>
+      <c r="AN11" t="inlineStr"/>
+      <c r="AO11" t="inlineStr"/>
+      <c r="AP11" t="inlineStr"/>
+      <c r="AQ11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
@@ -1859,7 +2069,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_64ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_1/20200207_jorgejovicich_cimec_human_sub1_64ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -1970,6 +2180,20 @@
           <t>[]</t>
         </is>
       </c>
+      <c r="AD12" t="inlineStr"/>
+      <c r="AE12" t="inlineStr"/>
+      <c r="AF12" t="inlineStr"/>
+      <c r="AG12" t="inlineStr"/>
+      <c r="AH12" t="inlineStr"/>
+      <c r="AI12" t="inlineStr"/>
+      <c r="AJ12" t="inlineStr"/>
+      <c r="AK12" t="inlineStr"/>
+      <c r="AL12" t="inlineStr"/>
+      <c r="AM12" t="inlineStr"/>
+      <c r="AN12" t="inlineStr"/>
+      <c r="AO12" t="inlineStr"/>
+      <c r="AP12" t="inlineStr"/>
+      <c r="AQ12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
@@ -1987,7 +2211,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_20ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_20ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -2099,6 +2323,20 @@
  1526.8 1436.6 1383.4 1567.3 1873.4 1817.3 1163.2 1269.1]</t>
         </is>
       </c>
+      <c r="AD13" t="inlineStr"/>
+      <c r="AE13" t="inlineStr"/>
+      <c r="AF13" t="inlineStr"/>
+      <c r="AG13" t="inlineStr"/>
+      <c r="AH13" t="inlineStr"/>
+      <c r="AI13" t="inlineStr"/>
+      <c r="AJ13" t="inlineStr"/>
+      <c r="AK13" t="inlineStr"/>
+      <c r="AL13" t="inlineStr"/>
+      <c r="AM13" t="inlineStr"/>
+      <c r="AN13" t="inlineStr"/>
+      <c r="AO13" t="inlineStr"/>
+      <c r="AP13" t="inlineStr"/>
+      <c r="AQ13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
@@ -2116,7 +2354,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_64ch_t1map.nii.gz</t>
+          <t>20200207_jorgejovicich_cimec_human/subject_2/20200207_jorgejovicich_cimec_human_sub2_64ch_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -2222,6 +2460,20 @@
  1144.2 1255.1 1281.6 1298.7 1237.7 1198.8 1228.7 1224.5]</t>
         </is>
       </c>
+      <c r="AD14" t="inlineStr"/>
+      <c r="AE14" t="inlineStr"/>
+      <c r="AF14" t="inlineStr"/>
+      <c r="AG14" t="inlineStr"/>
+      <c r="AH14" t="inlineStr"/>
+      <c r="AI14" t="inlineStr"/>
+      <c r="AJ14" t="inlineStr"/>
+      <c r="AK14" t="inlineStr"/>
+      <c r="AL14" t="inlineStr"/>
+      <c r="AM14" t="inlineStr"/>
+      <c r="AN14" t="inlineStr"/>
+      <c r="AO14" t="inlineStr"/>
+      <c r="AP14" t="inlineStr"/>
+      <c r="AQ14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
@@ -2239,7 +2491,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>20200219_marcocastellaro_UniPD_human/20200219_marcocastellaro_UniPD_human_Complex_t1map.nii.gz</t>
+          <t>20200219_marcocastellaro_UniPD_human/20200219_marcocastellaro_UniPD_human_Complex_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -2349,6 +2601,20 @@
  1364.5 1665.5 1438.9 1359.4 1679.5 1397.5 1297.3]</t>
         </is>
       </c>
+      <c r="AD15" t="inlineStr"/>
+      <c r="AE15" t="inlineStr"/>
+      <c r="AF15" t="inlineStr"/>
+      <c r="AG15" t="inlineStr"/>
+      <c r="AH15" t="inlineStr"/>
+      <c r="AI15" t="inlineStr"/>
+      <c r="AJ15" t="inlineStr"/>
+      <c r="AK15" t="inlineStr"/>
+      <c r="AL15" t="inlineStr"/>
+      <c r="AM15" t="inlineStr"/>
+      <c r="AN15" t="inlineStr"/>
+      <c r="AO15" t="inlineStr"/>
+      <c r="AP15" t="inlineStr"/>
+      <c r="AQ15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
@@ -2366,7 +2632,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>20200221_madelinecarr_lha_human/20200221_madelinecarr_lha_human_t1map.nii.gz</t>
+          <t>20200221_madelinecarr_lha_human/20200221_madelinecarr_lha_human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -2472,6 +2738,20 @@
  1344.2 1544.2]</t>
         </is>
       </c>
+      <c r="AD16" t="inlineStr"/>
+      <c r="AE16" t="inlineStr"/>
+      <c r="AF16" t="inlineStr"/>
+      <c r="AG16" t="inlineStr"/>
+      <c r="AH16" t="inlineStr"/>
+      <c r="AI16" t="inlineStr"/>
+      <c r="AJ16" t="inlineStr"/>
+      <c r="AK16" t="inlineStr"/>
+      <c r="AL16" t="inlineStr"/>
+      <c r="AM16" t="inlineStr"/>
+      <c r="AN16" t="inlineStr"/>
+      <c r="AO16" t="inlineStr"/>
+      <c r="AP16" t="inlineStr"/>
+      <c r="AQ16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
@@ -2489,7 +2769,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_magnitude_t1map.nii.gz</t>
+          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_magnitude_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -2596,6 +2876,20 @@
  1113.3 1249.9 1228.1 1308.6 1218.9 1309.4 1220.6 1249.1]</t>
         </is>
       </c>
+      <c r="AD17" t="inlineStr"/>
+      <c r="AE17" t="inlineStr"/>
+      <c r="AF17" t="inlineStr"/>
+      <c r="AG17" t="inlineStr"/>
+      <c r="AH17" t="inlineStr"/>
+      <c r="AI17" t="inlineStr"/>
+      <c r="AJ17" t="inlineStr"/>
+      <c r="AK17" t="inlineStr"/>
+      <c r="AL17" t="inlineStr"/>
+      <c r="AM17" t="inlineStr"/>
+      <c r="AN17" t="inlineStr"/>
+      <c r="AO17" t="inlineStr"/>
+      <c r="AP17" t="inlineStr"/>
+      <c r="AQ17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
@@ -2613,7 +2907,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_Complex_t1map.nii.gz</t>
+          <t>20200225_CStehningPhilipsClinicalScienceGermany_human/Hamburg_MR1_InVivo_Complex_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -2720,6 +3014,20 @@
  1095.8 1281.5 1186.6 1278.1 1185.7 1324.1 1227.8 1243.6]</t>
         </is>
       </c>
+      <c r="AD18" t="inlineStr"/>
+      <c r="AE18" t="inlineStr"/>
+      <c r="AF18" t="inlineStr"/>
+      <c r="AG18" t="inlineStr"/>
+      <c r="AH18" t="inlineStr"/>
+      <c r="AI18" t="inlineStr"/>
+      <c r="AJ18" t="inlineStr"/>
+      <c r="AK18" t="inlineStr"/>
+      <c r="AL18" t="inlineStr"/>
+      <c r="AM18" t="inlineStr"/>
+      <c r="AN18" t="inlineStr"/>
+      <c r="AO18" t="inlineStr"/>
+      <c r="AP18" t="inlineStr"/>
+      <c r="AQ18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
@@ -2737,7 +3045,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200206_190116_Ph/21527_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200206_190116_Ph/21527_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -2847,6 +3155,20 @@
  1391.7 1387.9 1433.5 1428.  1414.6 1411.5 1439.1]</t>
         </is>
       </c>
+      <c r="AD19" t="inlineStr"/>
+      <c r="AE19" t="inlineStr"/>
+      <c r="AF19" t="inlineStr"/>
+      <c r="AG19" t="inlineStr"/>
+      <c r="AH19" t="inlineStr"/>
+      <c r="AI19" t="inlineStr"/>
+      <c r="AJ19" t="inlineStr"/>
+      <c r="AK19" t="inlineStr"/>
+      <c r="AL19" t="inlineStr"/>
+      <c r="AM19" t="inlineStr"/>
+      <c r="AN19" t="inlineStr"/>
+      <c r="AO19" t="inlineStr"/>
+      <c r="AP19" t="inlineStr"/>
+      <c r="AQ19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
@@ -2864,7 +3186,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -2974,6 +3296,20 @@
  1547.9 1469.3 1431.  1418.6 1651.9 1628.8 1677.9]</t>
         </is>
       </c>
+      <c r="AD20" t="inlineStr"/>
+      <c r="AE20" t="inlineStr"/>
+      <c r="AF20" t="inlineStr"/>
+      <c r="AG20" t="inlineStr"/>
+      <c r="AH20" t="inlineStr"/>
+      <c r="AI20" t="inlineStr"/>
+      <c r="AJ20" t="inlineStr"/>
+      <c r="AK20" t="inlineStr"/>
+      <c r="AL20" t="inlineStr"/>
+      <c r="AM20" t="inlineStr"/>
+      <c r="AN20" t="inlineStr"/>
+      <c r="AO20" t="inlineStr"/>
+      <c r="AP20" t="inlineStr"/>
+      <c r="AQ20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
@@ -2991,7 +3327,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200120_191941_GE/21527_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -3101,6 +3437,20 @@
  1557.5 1466.9 1446.6 1421.9 1607.6 1585.5 1635.1]</t>
         </is>
       </c>
+      <c r="AD21" t="inlineStr"/>
+      <c r="AE21" t="inlineStr"/>
+      <c r="AF21" t="inlineStr"/>
+      <c r="AG21" t="inlineStr"/>
+      <c r="AH21" t="inlineStr"/>
+      <c r="AI21" t="inlineStr"/>
+      <c r="AJ21" t="inlineStr"/>
+      <c r="AK21" t="inlineStr"/>
+      <c r="AL21" t="inlineStr"/>
+      <c r="AM21" t="inlineStr"/>
+      <c r="AN21" t="inlineStr"/>
+      <c r="AO21" t="inlineStr"/>
+      <c r="AP21" t="inlineStr"/>
+      <c r="AQ21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
@@ -3118,7 +3468,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -3228,6 +3578,20 @@
  1457.8 1493.9 1555.6 1600.6 1492.3 1653.6 1682.7]</t>
         </is>
       </c>
+      <c r="AD22" t="inlineStr"/>
+      <c r="AE22" t="inlineStr"/>
+      <c r="AF22" t="inlineStr"/>
+      <c r="AG22" t="inlineStr"/>
+      <c r="AH22" t="inlineStr"/>
+      <c r="AI22" t="inlineStr"/>
+      <c r="AJ22" t="inlineStr"/>
+      <c r="AK22" t="inlineStr"/>
+      <c r="AL22" t="inlineStr"/>
+      <c r="AM22" t="inlineStr"/>
+      <c r="AN22" t="inlineStr"/>
+      <c r="AO22" t="inlineStr"/>
+      <c r="AP22" t="inlineStr"/>
+      <c r="AQ22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
@@ -3245,7 +3609,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/21527/20200124_120146_GE/21527_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -3355,6 +3719,20 @@
  1460.5 1499.1 1568.8 1603.8 1544.2 1650.3 1677.6]</t>
         </is>
       </c>
+      <c r="AD23" t="inlineStr"/>
+      <c r="AE23" t="inlineStr"/>
+      <c r="AF23" t="inlineStr"/>
+      <c r="AG23" t="inlineStr"/>
+      <c r="AH23" t="inlineStr"/>
+      <c r="AI23" t="inlineStr"/>
+      <c r="AJ23" t="inlineStr"/>
+      <c r="AK23" t="inlineStr"/>
+      <c r="AL23" t="inlineStr"/>
+      <c r="AM23" t="inlineStr"/>
+      <c r="AN23" t="inlineStr"/>
+      <c r="AO23" t="inlineStr"/>
+      <c r="AP23" t="inlineStr"/>
+      <c r="AQ23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
@@ -3372,7 +3750,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -3482,6 +3860,20 @@
  1435.  1599.7 1631.4 1496.7 1490.7 1506.3 1539.9]</t>
         </is>
       </c>
+      <c r="AD24" t="inlineStr"/>
+      <c r="AE24" t="inlineStr"/>
+      <c r="AF24" t="inlineStr"/>
+      <c r="AG24" t="inlineStr"/>
+      <c r="AH24" t="inlineStr"/>
+      <c r="AI24" t="inlineStr"/>
+      <c r="AJ24" t="inlineStr"/>
+      <c r="AK24" t="inlineStr"/>
+      <c r="AL24" t="inlineStr"/>
+      <c r="AM24" t="inlineStr"/>
+      <c r="AN24" t="inlineStr"/>
+      <c r="AO24" t="inlineStr"/>
+      <c r="AP24" t="inlineStr"/>
+      <c r="AQ24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
@@ -3499,7 +3891,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_153220_GE/56190_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -3609,6 +4001,20 @@
  1476.5 1551.  1579.1 1505.9 1458.5 1468.2 1535.3]</t>
         </is>
       </c>
+      <c r="AD25" t="inlineStr"/>
+      <c r="AE25" t="inlineStr"/>
+      <c r="AF25" t="inlineStr"/>
+      <c r="AG25" t="inlineStr"/>
+      <c r="AH25" t="inlineStr"/>
+      <c r="AI25" t="inlineStr"/>
+      <c r="AJ25" t="inlineStr"/>
+      <c r="AK25" t="inlineStr"/>
+      <c r="AL25" t="inlineStr"/>
+      <c r="AM25" t="inlineStr"/>
+      <c r="AN25" t="inlineStr"/>
+      <c r="AO25" t="inlineStr"/>
+      <c r="AP25" t="inlineStr"/>
+      <c r="AQ25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
@@ -3626,7 +4032,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_151000_Ph/56190_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56190/20200223_151000_Ph/56190_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -3735,6 +4141,20 @@
  1511.4 1462.2 1429.5 1446.7 1445.2 1348.9 1296.2 1384. ]</t>
         </is>
       </c>
+      <c r="AD26" t="inlineStr"/>
+      <c r="AE26" t="inlineStr"/>
+      <c r="AF26" t="inlineStr"/>
+      <c r="AG26" t="inlineStr"/>
+      <c r="AH26" t="inlineStr"/>
+      <c r="AI26" t="inlineStr"/>
+      <c r="AJ26" t="inlineStr"/>
+      <c r="AK26" t="inlineStr"/>
+      <c r="AL26" t="inlineStr"/>
+      <c r="AM26" t="inlineStr"/>
+      <c r="AN26" t="inlineStr"/>
+      <c r="AO26" t="inlineStr"/>
+      <c r="AP26" t="inlineStr"/>
+      <c r="AQ26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
@@ -3752,7 +4172,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -3862,6 +4282,20 @@
  1833.5 1454.2 1577.6 1591.6 1396.6 1497.2 1486.9]</t>
         </is>
       </c>
+      <c r="AD27" t="inlineStr"/>
+      <c r="AE27" t="inlineStr"/>
+      <c r="AF27" t="inlineStr"/>
+      <c r="AG27" t="inlineStr"/>
+      <c r="AH27" t="inlineStr"/>
+      <c r="AI27" t="inlineStr"/>
+      <c r="AJ27" t="inlineStr"/>
+      <c r="AK27" t="inlineStr"/>
+      <c r="AL27" t="inlineStr"/>
+      <c r="AM27" t="inlineStr"/>
+      <c r="AN27" t="inlineStr"/>
+      <c r="AO27" t="inlineStr"/>
+      <c r="AP27" t="inlineStr"/>
+      <c r="AQ27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
@@ -3879,7 +4313,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_135500_GE/56961_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -3989,6 +4423,20 @@
  1810.3 1442.7 1577.  1600.2 1382.4 1470.  1487.6]</t>
         </is>
       </c>
+      <c r="AD28" t="inlineStr"/>
+      <c r="AE28" t="inlineStr"/>
+      <c r="AF28" t="inlineStr"/>
+      <c r="AG28" t="inlineStr"/>
+      <c r="AH28" t="inlineStr"/>
+      <c r="AI28" t="inlineStr"/>
+      <c r="AJ28" t="inlineStr"/>
+      <c r="AK28" t="inlineStr"/>
+      <c r="AL28" t="inlineStr"/>
+      <c r="AM28" t="inlineStr"/>
+      <c r="AN28" t="inlineStr"/>
+      <c r="AO28" t="inlineStr"/>
+      <c r="AP28" t="inlineStr"/>
+      <c r="AQ28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
@@ -4006,7 +4454,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_133135_Ph/56961_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56961/20200223_133135_Ph/56961_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -4112,6 +4560,20 @@
  1518.9 1444.3 1251.4 1141.8 1403.7 1232.  1563.8 1386.9]</t>
         </is>
       </c>
+      <c r="AD29" t="inlineStr"/>
+      <c r="AE29" t="inlineStr"/>
+      <c r="AF29" t="inlineStr"/>
+      <c r="AG29" t="inlineStr"/>
+      <c r="AH29" t="inlineStr"/>
+      <c r="AI29" t="inlineStr"/>
+      <c r="AJ29" t="inlineStr"/>
+      <c r="AK29" t="inlineStr"/>
+      <c r="AL29" t="inlineStr"/>
+      <c r="AM29" t="inlineStr"/>
+      <c r="AN29" t="inlineStr"/>
+      <c r="AO29" t="inlineStr"/>
+      <c r="AP29" t="inlineStr"/>
+      <c r="AQ29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
@@ -4129,7 +4591,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_141051_Ph/58416_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_141051_Ph/58416_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -4239,6 +4701,20 @@
  1678.1 1732.  1776.9 1759.3 1766.8 1758.8 1862.8]</t>
         </is>
       </c>
+      <c r="AD30" t="inlineStr"/>
+      <c r="AE30" t="inlineStr"/>
+      <c r="AF30" t="inlineStr"/>
+      <c r="AG30" t="inlineStr"/>
+      <c r="AH30" t="inlineStr"/>
+      <c r="AI30" t="inlineStr"/>
+      <c r="AJ30" t="inlineStr"/>
+      <c r="AK30" t="inlineStr"/>
+      <c r="AL30" t="inlineStr"/>
+      <c r="AM30" t="inlineStr"/>
+      <c r="AN30" t="inlineStr"/>
+      <c r="AO30" t="inlineStr"/>
+      <c r="AP30" t="inlineStr"/>
+      <c r="AQ30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
@@ -4256,7 +4732,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -4366,6 +4842,20 @@
  1552.5 1596.1 1644.6 1711.  1463.8 1487.3 1561.3]</t>
         </is>
       </c>
+      <c r="AD31" t="inlineStr"/>
+      <c r="AE31" t="inlineStr"/>
+      <c r="AF31" t="inlineStr"/>
+      <c r="AG31" t="inlineStr"/>
+      <c r="AH31" t="inlineStr"/>
+      <c r="AI31" t="inlineStr"/>
+      <c r="AJ31" t="inlineStr"/>
+      <c r="AK31" t="inlineStr"/>
+      <c r="AL31" t="inlineStr"/>
+      <c r="AM31" t="inlineStr"/>
+      <c r="AN31" t="inlineStr"/>
+      <c r="AO31" t="inlineStr"/>
+      <c r="AP31" t="inlineStr"/>
+      <c r="AQ31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
@@ -4383,7 +4873,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58416/20200223_144142_GE/58416_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -4493,6 +4983,20 @@
  1520.9 1588.  1658.3 1740.9 1444.8 1501.9 1645.5]</t>
         </is>
       </c>
+      <c r="AD32" t="inlineStr"/>
+      <c r="AE32" t="inlineStr"/>
+      <c r="AF32" t="inlineStr"/>
+      <c r="AG32" t="inlineStr"/>
+      <c r="AH32" t="inlineStr"/>
+      <c r="AI32" t="inlineStr"/>
+      <c r="AJ32" t="inlineStr"/>
+      <c r="AK32" t="inlineStr"/>
+      <c r="AL32" t="inlineStr"/>
+      <c r="AM32" t="inlineStr"/>
+      <c r="AN32" t="inlineStr"/>
+      <c r="AO32" t="inlineStr"/>
+      <c r="AP32" t="inlineStr"/>
+      <c r="AQ32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
@@ -4510,7 +5014,7 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_145118_Ph/58139_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_145118_Ph/58139_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
@@ -4616,6 +5120,20 @@
  1686.4 1607.5 1561.4 1633.2 1703.9 1696.5 1751.7 1621.8]</t>
         </is>
       </c>
+      <c r="AD33" t="inlineStr"/>
+      <c r="AE33" t="inlineStr"/>
+      <c r="AF33" t="inlineStr"/>
+      <c r="AG33" t="inlineStr"/>
+      <c r="AH33" t="inlineStr"/>
+      <c r="AI33" t="inlineStr"/>
+      <c r="AJ33" t="inlineStr"/>
+      <c r="AK33" t="inlineStr"/>
+      <c r="AL33" t="inlineStr"/>
+      <c r="AM33" t="inlineStr"/>
+      <c r="AN33" t="inlineStr"/>
+      <c r="AO33" t="inlineStr"/>
+      <c r="AP33" t="inlineStr"/>
+      <c r="AQ33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
@@ -4633,7 +5151,7 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
@@ -4743,6 +5261,20 @@
  1736.7 1422.4 1488.7 1722.2 1488.9 1563.1 1694.2]</t>
         </is>
       </c>
+      <c r="AD34" t="inlineStr"/>
+      <c r="AE34" t="inlineStr"/>
+      <c r="AF34" t="inlineStr"/>
+      <c r="AG34" t="inlineStr"/>
+      <c r="AH34" t="inlineStr"/>
+      <c r="AI34" t="inlineStr"/>
+      <c r="AJ34" t="inlineStr"/>
+      <c r="AK34" t="inlineStr"/>
+      <c r="AL34" t="inlineStr"/>
+      <c r="AM34" t="inlineStr"/>
+      <c r="AN34" t="inlineStr"/>
+      <c r="AO34" t="inlineStr"/>
+      <c r="AP34" t="inlineStr"/>
+      <c r="AQ34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
@@ -4760,7 +5292,7 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58139/20200223_133141_GE/58139_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
@@ -4870,6 +5402,20 @@
  1691.1 1483.4 1526.1 1666.9 1525.3 1575.  1658.8]</t>
         </is>
       </c>
+      <c r="AD35" t="inlineStr"/>
+      <c r="AE35" t="inlineStr"/>
+      <c r="AF35" t="inlineStr"/>
+      <c r="AG35" t="inlineStr"/>
+      <c r="AH35" t="inlineStr"/>
+      <c r="AI35" t="inlineStr"/>
+      <c r="AJ35" t="inlineStr"/>
+      <c r="AK35" t="inlineStr"/>
+      <c r="AL35" t="inlineStr"/>
+      <c r="AM35" t="inlineStr"/>
+      <c r="AN35" t="inlineStr"/>
+      <c r="AO35" t="inlineStr"/>
+      <c r="AP35" t="inlineStr"/>
+      <c r="AQ35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
@@ -4887,7 +5433,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58173/20200206_182142_Ph/58173_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58173/20200206_182142_Ph/58173_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -4997,6 +5543,20 @@
  1586.2 1706.5 1903.8 1716.4 1622.5 1660.6 1766.8]</t>
         </is>
       </c>
+      <c r="AD36" t="inlineStr"/>
+      <c r="AE36" t="inlineStr"/>
+      <c r="AF36" t="inlineStr"/>
+      <c r="AG36" t="inlineStr"/>
+      <c r="AH36" t="inlineStr"/>
+      <c r="AI36" t="inlineStr"/>
+      <c r="AJ36" t="inlineStr"/>
+      <c r="AK36" t="inlineStr"/>
+      <c r="AL36" t="inlineStr"/>
+      <c r="AM36" t="inlineStr"/>
+      <c r="AN36" t="inlineStr"/>
+      <c r="AO36" t="inlineStr"/>
+      <c r="AP36" t="inlineStr"/>
+      <c r="AQ36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
@@ -5014,7 +5574,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58174/20200206_184031_Ph/58174_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58174/20200206_184031_Ph/58174_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -5120,6 +5680,20 @@
  1763.4 1679.8 1748.5 1610.3 1446.4 2015.2 1639.9 1573.5]</t>
         </is>
       </c>
+      <c r="AD37" t="inlineStr"/>
+      <c r="AE37" t="inlineStr"/>
+      <c r="AF37" t="inlineStr"/>
+      <c r="AG37" t="inlineStr"/>
+      <c r="AH37" t="inlineStr"/>
+      <c r="AI37" t="inlineStr"/>
+      <c r="AJ37" t="inlineStr"/>
+      <c r="AK37" t="inlineStr"/>
+      <c r="AL37" t="inlineStr"/>
+      <c r="AM37" t="inlineStr"/>
+      <c r="AN37" t="inlineStr"/>
+      <c r="AO37" t="inlineStr"/>
+      <c r="AP37" t="inlineStr"/>
+      <c r="AQ37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
@@ -5137,7 +5711,7 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
@@ -5247,6 +5821,20 @@
  1274.9 1399.  1272.8 1258.9 1379.6 1242.5 1221.4]</t>
         </is>
       </c>
+      <c r="AD38" t="inlineStr"/>
+      <c r="AE38" t="inlineStr"/>
+      <c r="AF38" t="inlineStr"/>
+      <c r="AG38" t="inlineStr"/>
+      <c r="AH38" t="inlineStr"/>
+      <c r="AI38" t="inlineStr"/>
+      <c r="AJ38" t="inlineStr"/>
+      <c r="AK38" t="inlineStr"/>
+      <c r="AL38" t="inlineStr"/>
+      <c r="AM38" t="inlineStr"/>
+      <c r="AN38" t="inlineStr"/>
+      <c r="AO38" t="inlineStr"/>
+      <c r="AP38" t="inlineStr"/>
+      <c r="AQ38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
@@ -5264,7 +5852,7 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_130855_GE/58414_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
@@ -5374,6 +5962,20 @@
  1300.6 1409.2 1277.4 1279.4 1361.6 1230.4 1239.2]</t>
         </is>
       </c>
+      <c r="AD39" t="inlineStr"/>
+      <c r="AE39" t="inlineStr"/>
+      <c r="AF39" t="inlineStr"/>
+      <c r="AG39" t="inlineStr"/>
+      <c r="AH39" t="inlineStr"/>
+      <c r="AI39" t="inlineStr"/>
+      <c r="AJ39" t="inlineStr"/>
+      <c r="AK39" t="inlineStr"/>
+      <c r="AL39" t="inlineStr"/>
+      <c r="AM39" t="inlineStr"/>
+      <c r="AN39" t="inlineStr"/>
+      <c r="AO39" t="inlineStr"/>
+      <c r="AP39" t="inlineStr"/>
+      <c r="AQ39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
@@ -5391,7 +5993,7 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_124551_Ph/58414_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58414/20200223_124551_Ph/58414_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
@@ -5501,6 +6103,20 @@
  1407.2 1457.9 1493.6 1411.3 1459.5 1442.8 1425.1]</t>
         </is>
       </c>
+      <c r="AD40" t="inlineStr"/>
+      <c r="AE40" t="inlineStr"/>
+      <c r="AF40" t="inlineStr"/>
+      <c r="AG40" t="inlineStr"/>
+      <c r="AH40" t="inlineStr"/>
+      <c r="AI40" t="inlineStr"/>
+      <c r="AJ40" t="inlineStr"/>
+      <c r="AK40" t="inlineStr"/>
+      <c r="AL40" t="inlineStr"/>
+      <c r="AM40" t="inlineStr"/>
+      <c r="AN40" t="inlineStr"/>
+      <c r="AO40" t="inlineStr"/>
+      <c r="AP40" t="inlineStr"/>
+      <c r="AQ40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
@@ -5518,7 +6134,7 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
@@ -5628,6 +6244,20 @@
  1474.6 1577.4 1558.6 1510.1 1686.  1666.9 1622.6]</t>
         </is>
       </c>
+      <c r="AD41" t="inlineStr"/>
+      <c r="AE41" t="inlineStr"/>
+      <c r="AF41" t="inlineStr"/>
+      <c r="AG41" t="inlineStr"/>
+      <c r="AH41" t="inlineStr"/>
+      <c r="AI41" t="inlineStr"/>
+      <c r="AJ41" t="inlineStr"/>
+      <c r="AK41" t="inlineStr"/>
+      <c r="AL41" t="inlineStr"/>
+      <c r="AM41" t="inlineStr"/>
+      <c r="AN41" t="inlineStr"/>
+      <c r="AO41" t="inlineStr"/>
+      <c r="AP41" t="inlineStr"/>
+      <c r="AQ41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
@@ -5645,7 +6275,7 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_122559_GE/58413_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
@@ -5755,6 +6385,20 @@
  1452.7 1583.3 1536.6 1499.6 1617.  1602.7 1578. ]</t>
         </is>
       </c>
+      <c r="AD42" t="inlineStr"/>
+      <c r="AE42" t="inlineStr"/>
+      <c r="AF42" t="inlineStr"/>
+      <c r="AG42" t="inlineStr"/>
+      <c r="AH42" t="inlineStr"/>
+      <c r="AI42" t="inlineStr"/>
+      <c r="AJ42" t="inlineStr"/>
+      <c r="AK42" t="inlineStr"/>
+      <c r="AL42" t="inlineStr"/>
+      <c r="AM42" t="inlineStr"/>
+      <c r="AN42" t="inlineStr"/>
+      <c r="AO42" t="inlineStr"/>
+      <c r="AP42" t="inlineStr"/>
+      <c r="AQ42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
@@ -5772,7 +6416,7 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
@@ -5882,6 +6526,20 @@
  1838.  2013.8 2122.  1784.  1677.  1781.9 1888.8]</t>
         </is>
       </c>
+      <c r="AD43" t="inlineStr"/>
+      <c r="AE43" t="inlineStr"/>
+      <c r="AF43" t="inlineStr"/>
+      <c r="AG43" t="inlineStr"/>
+      <c r="AH43" t="inlineStr"/>
+      <c r="AI43" t="inlineStr"/>
+      <c r="AJ43" t="inlineStr"/>
+      <c r="AK43" t="inlineStr"/>
+      <c r="AL43" t="inlineStr"/>
+      <c r="AM43" t="inlineStr"/>
+      <c r="AN43" t="inlineStr"/>
+      <c r="AO43" t="inlineStr"/>
+      <c r="AP43" t="inlineStr"/>
+      <c r="AQ43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
@@ -5899,7 +6557,7 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData-2_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58413/20200223_131003_Ph/58413_Ph_mag_IRData-2_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
@@ -6009,6 +6667,20 @@
  1835.9 1865.6 2013.6 1803.  1526.6 1683.7 1892.3]</t>
         </is>
       </c>
+      <c r="AD44" t="inlineStr"/>
+      <c r="AE44" t="inlineStr"/>
+      <c r="AF44" t="inlineStr"/>
+      <c r="AG44" t="inlineStr"/>
+      <c r="AH44" t="inlineStr"/>
+      <c r="AI44" t="inlineStr"/>
+      <c r="AJ44" t="inlineStr"/>
+      <c r="AK44" t="inlineStr"/>
+      <c r="AL44" t="inlineStr"/>
+      <c r="AM44" t="inlineStr"/>
+      <c r="AN44" t="inlineStr"/>
+      <c r="AO44" t="inlineStr"/>
+      <c r="AP44" t="inlineStr"/>
+      <c r="AQ44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
@@ -6026,7 +6698,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -6136,6 +6808,20 @@
  1392.9 1460.9 1382.6 1455.  1469.6 1379.2 1452. ]</t>
         </is>
       </c>
+      <c r="AD45" t="inlineStr"/>
+      <c r="AE45" t="inlineStr"/>
+      <c r="AF45" t="inlineStr"/>
+      <c r="AG45" t="inlineStr"/>
+      <c r="AH45" t="inlineStr"/>
+      <c r="AI45" t="inlineStr"/>
+      <c r="AJ45" t="inlineStr"/>
+      <c r="AK45" t="inlineStr"/>
+      <c r="AL45" t="inlineStr"/>
+      <c r="AM45" t="inlineStr"/>
+      <c r="AN45" t="inlineStr"/>
+      <c r="AO45" t="inlineStr"/>
+      <c r="AP45" t="inlineStr"/>
+      <c r="AQ45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
@@ -6153,7 +6839,7 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_155637_GE/56347_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
@@ -6263,6 +6949,20 @@
  1401.5 1459.  1405.  1444.7 1466.  1402.5 1439.7]</t>
         </is>
       </c>
+      <c r="AD46" t="inlineStr"/>
+      <c r="AE46" t="inlineStr"/>
+      <c r="AF46" t="inlineStr"/>
+      <c r="AG46" t="inlineStr"/>
+      <c r="AH46" t="inlineStr"/>
+      <c r="AI46" t="inlineStr"/>
+      <c r="AJ46" t="inlineStr"/>
+      <c r="AK46" t="inlineStr"/>
+      <c r="AL46" t="inlineStr"/>
+      <c r="AM46" t="inlineStr"/>
+      <c r="AN46" t="inlineStr"/>
+      <c r="AO46" t="inlineStr"/>
+      <c r="AP46" t="inlineStr"/>
+      <c r="AQ46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
@@ -6280,7 +6980,7 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_152800_Ph/56347_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56347/20200223_152800_Ph/56347_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
@@ -6386,6 +7086,20 @@
  1705.6 1758.3 1563.3 1524.6 1712.9 1687.8 1720.  1678.4]</t>
         </is>
       </c>
+      <c r="AD47" t="inlineStr"/>
+      <c r="AE47" t="inlineStr"/>
+      <c r="AF47" t="inlineStr"/>
+      <c r="AG47" t="inlineStr"/>
+      <c r="AH47" t="inlineStr"/>
+      <c r="AI47" t="inlineStr"/>
+      <c r="AJ47" t="inlineStr"/>
+      <c r="AK47" t="inlineStr"/>
+      <c r="AL47" t="inlineStr"/>
+      <c r="AM47" t="inlineStr"/>
+      <c r="AN47" t="inlineStr"/>
+      <c r="AO47" t="inlineStr"/>
+      <c r="AP47" t="inlineStr"/>
+      <c r="AQ47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
@@ -6403,7 +7117,7 @@
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_134934_Ph/58415_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_134934_Ph/58415_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
@@ -6513,6 +7227,20 @@
  1503.  1626.2 1574.2 1626.4 1544.4 1528.4 1530. ]</t>
         </is>
       </c>
+      <c r="AD48" t="inlineStr"/>
+      <c r="AE48" t="inlineStr"/>
+      <c r="AF48" t="inlineStr"/>
+      <c r="AG48" t="inlineStr"/>
+      <c r="AH48" t="inlineStr"/>
+      <c r="AI48" t="inlineStr"/>
+      <c r="AJ48" t="inlineStr"/>
+      <c r="AK48" t="inlineStr"/>
+      <c r="AL48" t="inlineStr"/>
+      <c r="AM48" t="inlineStr"/>
+      <c r="AN48" t="inlineStr"/>
+      <c r="AO48" t="inlineStr"/>
+      <c r="AP48" t="inlineStr"/>
+      <c r="AQ48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
@@ -6530,7 +7258,7 @@
       </c>
       <c r="D49" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E49" t="inlineStr">
@@ -6640,6 +7368,20 @@
  1638.6 1542.1 1658.  1625.8 1585.3 1648.4 1511.2]</t>
         </is>
       </c>
+      <c r="AD49" t="inlineStr"/>
+      <c r="AE49" t="inlineStr"/>
+      <c r="AF49" t="inlineStr"/>
+      <c r="AG49" t="inlineStr"/>
+      <c r="AH49" t="inlineStr"/>
+      <c r="AI49" t="inlineStr"/>
+      <c r="AJ49" t="inlineStr"/>
+      <c r="AK49" t="inlineStr"/>
+      <c r="AL49" t="inlineStr"/>
+      <c r="AM49" t="inlineStr"/>
+      <c r="AN49" t="inlineStr"/>
+      <c r="AO49" t="inlineStr"/>
+      <c r="AP49" t="inlineStr"/>
+      <c r="AQ49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
@@ -6657,7 +7399,7 @@
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58415/20200223_142008_GE/58415_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
@@ -6767,6 +7509,20 @@
  1684.2 1517.5 1683.2 1646.2 1577.6 1671.7 1506.6]</t>
         </is>
       </c>
+      <c r="AD50" t="inlineStr"/>
+      <c r="AE50" t="inlineStr"/>
+      <c r="AF50" t="inlineStr"/>
+      <c r="AG50" t="inlineStr"/>
+      <c r="AH50" t="inlineStr"/>
+      <c r="AI50" t="inlineStr"/>
+      <c r="AJ50" t="inlineStr"/>
+      <c r="AK50" t="inlineStr"/>
+      <c r="AL50" t="inlineStr"/>
+      <c r="AM50" t="inlineStr"/>
+      <c r="AN50" t="inlineStr"/>
+      <c r="AO50" t="inlineStr"/>
+      <c r="AP50" t="inlineStr"/>
+      <c r="AQ50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
@@ -6784,7 +7540,7 @@
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
@@ -6894,6 +7650,20 @@
  1518.  1544.2 1594.1 1614.8 1481.8 1674.6 1589.2]</t>
         </is>
       </c>
+      <c r="AD51" t="inlineStr"/>
+      <c r="AE51" t="inlineStr"/>
+      <c r="AF51" t="inlineStr"/>
+      <c r="AG51" t="inlineStr"/>
+      <c r="AH51" t="inlineStr"/>
+      <c r="AI51" t="inlineStr"/>
+      <c r="AJ51" t="inlineStr"/>
+      <c r="AK51" t="inlineStr"/>
+      <c r="AL51" t="inlineStr"/>
+      <c r="AM51" t="inlineStr"/>
+      <c r="AN51" t="inlineStr"/>
+      <c r="AO51" t="inlineStr"/>
+      <c r="AP51" t="inlineStr"/>
+      <c r="AQ51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
@@ -6911,7 +7681,7 @@
       </c>
       <c r="D52" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_124731_GE/56348_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E52" t="inlineStr">
@@ -7021,6 +7791,20 @@
  1547.4 1568.3 1549.8 1611.1 1482.1 1585.8 1571.8]</t>
         </is>
       </c>
+      <c r="AD52" t="inlineStr"/>
+      <c r="AE52" t="inlineStr"/>
+      <c r="AF52" t="inlineStr"/>
+      <c r="AG52" t="inlineStr"/>
+      <c r="AH52" t="inlineStr"/>
+      <c r="AI52" t="inlineStr"/>
+      <c r="AJ52" t="inlineStr"/>
+      <c r="AK52" t="inlineStr"/>
+      <c r="AL52" t="inlineStr"/>
+      <c r="AM52" t="inlineStr"/>
+      <c r="AN52" t="inlineStr"/>
+      <c r="AO52" t="inlineStr"/>
+      <c r="AP52" t="inlineStr"/>
+      <c r="AQ52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
@@ -7038,7 +7822,7 @@
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_122504_Ph/56348_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/56348/20200223_122504_Ph/56348_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
@@ -7146,6 +7930,20 @@
           <t>[1895.6 1749.3 1537.6 1722.9 1646.6 1513.6 1669.3 1714.6 1763. ]</t>
         </is>
       </c>
+      <c r="AD53" t="inlineStr"/>
+      <c r="AE53" t="inlineStr"/>
+      <c r="AF53" t="inlineStr"/>
+      <c r="AG53" t="inlineStr"/>
+      <c r="AH53" t="inlineStr"/>
+      <c r="AI53" t="inlineStr"/>
+      <c r="AJ53" t="inlineStr"/>
+      <c r="AK53" t="inlineStr"/>
+      <c r="AL53" t="inlineStr"/>
+      <c r="AM53" t="inlineStr"/>
+      <c r="AN53" t="inlineStr"/>
+      <c r="AO53" t="inlineStr"/>
+      <c r="AP53" t="inlineStr"/>
+      <c r="AQ53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
@@ -7163,7 +7961,7 @@
       </c>
       <c r="D54" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_142721_Ph/58132_Ph_mag_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_142721_Ph/58132_Ph_mag_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E54" t="inlineStr">
@@ -7269,6 +8067,20 @@
  2027.4 2185.3 1878.8 1770.9 1804.8 1723.6 1783.6 1717.1]</t>
         </is>
       </c>
+      <c r="AD54" t="inlineStr"/>
+      <c r="AE54" t="inlineStr"/>
+      <c r="AF54" t="inlineStr"/>
+      <c r="AG54" t="inlineStr"/>
+      <c r="AH54" t="inlineStr"/>
+      <c r="AI54" t="inlineStr"/>
+      <c r="AJ54" t="inlineStr"/>
+      <c r="AK54" t="inlineStr"/>
+      <c r="AL54" t="inlineStr"/>
+      <c r="AM54" t="inlineStr"/>
+      <c r="AN54" t="inlineStr"/>
+      <c r="AO54" t="inlineStr"/>
+      <c r="AP54" t="inlineStr"/>
+      <c r="AQ54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
@@ -7286,7 +8098,7 @@
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_raw_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_raw_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -7396,6 +8208,20 @@
  1437.8 1427.5 1364.7 1342.4 1438.3 1399.2 1408.7]</t>
         </is>
       </c>
+      <c r="AD55" t="inlineStr"/>
+      <c r="AE55" t="inlineStr"/>
+      <c r="AF55" t="inlineStr"/>
+      <c r="AG55" t="inlineStr"/>
+      <c r="AH55" t="inlineStr"/>
+      <c r="AI55" t="inlineStr"/>
+      <c r="AJ55" t="inlineStr"/>
+      <c r="AK55" t="inlineStr"/>
+      <c r="AL55" t="inlineStr"/>
+      <c r="AM55" t="inlineStr"/>
+      <c r="AN55" t="inlineStr"/>
+      <c r="AO55" t="inlineStr"/>
+      <c r="AP55" t="inlineStr"/>
+      <c r="AQ55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
@@ -7413,7 +8239,7 @@
       </c>
       <c r="D56" t="inlineStr">
         <is>
-          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_filtered_IRData_t1map.nii.gz</t>
+          <t>20200225_luisconcha_UNAM_human/session_1/58132/20200223_150602_GE/58132_GE_filtered_IRData_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E56" t="inlineStr">
@@ -7523,6 +8349,20 @@
  1476.5 1435.3 1399.5 1380.9 1426.3 1400.5 1398.4]</t>
         </is>
       </c>
+      <c r="AD56" t="inlineStr"/>
+      <c r="AE56" t="inlineStr"/>
+      <c r="AF56" t="inlineStr"/>
+      <c r="AG56" t="inlineStr"/>
+      <c r="AH56" t="inlineStr"/>
+      <c r="AI56" t="inlineStr"/>
+      <c r="AJ56" t="inlineStr"/>
+      <c r="AK56" t="inlineStr"/>
+      <c r="AL56" t="inlineStr"/>
+      <c r="AM56" t="inlineStr"/>
+      <c r="AN56" t="inlineStr"/>
+      <c r="AO56" t="inlineStr"/>
+      <c r="AP56" t="inlineStr"/>
+      <c r="AQ56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
@@ -7540,7 +8380,7 @@
       </c>
       <c r="D57" t="inlineStr">
         <is>
-          <t>20200226_iveslevesque_muhc_glen_human/20200226_muhc_glen_Human_t1map.nii.gz</t>
+          <t>20200226_iveslevesque_muhc_glen_human/20200226_muhc_glen_Human_T1map.nii.gz</t>
         </is>
       </c>
       <c r="E57" t="inlineStr">
@@ -7648,6 +8488,20 @@
  1446.1 1293.4 1344.  1424.6 1326.  1352.5 1399.1]</t>
         </is>
       </c>
+      <c r="AD57" t="inlineStr"/>
+      <c r="AE57" t="inlineStr"/>
+      <c r="AF57" t="inlineStr"/>
+      <c r="AG57" t="inlineStr"/>
+      <c r="AH57" t="inlineStr"/>
+      <c r="AI57" t="inlineStr"/>
+      <c r="AJ57" t="inlineStr"/>
+      <c r="AK57" t="inlineStr"/>
+      <c r="AL57" t="inlineStr"/>
+      <c r="AM57" t="inlineStr"/>
+      <c r="AN57" t="inlineStr"/>
+      <c r="AO57" t="inlineStr"/>
+      <c r="AP57" t="inlineStr"/>
+      <c r="AQ57" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
Update database for reuploaded ROIs of site 2.004 (ROI4 mislabeled as ROI3)
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -50,22 +50,21 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -1323,17 +1322,16 @@
       </c>
       <c r="AB6" t="inlineStr">
         <is>
-          <t>[1431.7 1392.1 1435.7 1384.8 1255.9 1371.4 1408.3 1266.5 1338.3 1320.2
- 1329.4 1345.5 1253.1 1310.8 1204.  1221.1 1314.5 1349.4 1375.  1382.4
- 1349.3 1358.3 1354.1 1344.5 1389.1 1491.2 1405.2 1286.6 1314.  1451.5
- 1488.  1398.2 1390.3 1487.5 1019.3  654.1 1193.  1431.9 1117.9 3170.
- 1440.7 1940.4 3290.6 1505.6 1615.6 1522.4 1506.5 1591.8 1704.7 1601.
- 1469.4 1567.8]</t>
+          <t>[1320.2 1329.4 1345.5 1253.1 1310.8 1204.  1221.1 1314.5 1349.4 1375.
+ 1382.4 1349.3 1358.3 1354.1 1344.5 1389.1 1491.2 1405.2 1286.6 1314.
+ 1451.5 1488.  1398.2 1390.3 1487.5]</t>
         </is>
       </c>
       <c r="AC6" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>[1431.7 1392.1 1435.7 1384.8 1255.9 1371.4 1408.3 1266.5 1338.3 1019.3
+  654.1 1193.  1431.9 1117.9 3170.  1440.7 1940.4 3290.6 1505.6 1615.6
+ 1522.4 1506.5 1591.8 1704.7 1601.  1469.4 1567.8]</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr"/>
@@ -8504,6 +8502,6 @@
       <c r="AQ57" t="inlineStr"/>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update database for reuploaded ROIs of site 2.004 (fixed some outlisers in ROI 4, CSF instead of cGM)
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -1330,8 +1330,8 @@
       <c r="AC6" t="inlineStr">
         <is>
           <t>[1431.7 1392.1 1435.7 1384.8 1255.9 1371.4 1408.3 1266.5 1338.3 1019.3
-  654.1 1193.  1431.9 1117.9 3170.  1440.7 1940.4 3290.6 1505.6 1615.6
- 1522.4 1506.5 1591.8 1704.7 1601.  1469.4 1567.8]</t>
+  654.1 1193.  1431.9 1117.9 1440.7 1940.4 1505.6 1615.6 1522.4 1506.5
+ 1591.8 1704.7 1601.  1469.4 1567.8]</t>
         </is>
       </c>
       <c r="AD6" t="inlineStr"/>

</xml_diff>

<commit_message>
Regenerate database with datasets https://osf.io/b2sm8/ (refaatgabr) and https://osf.io/n47jz/ (marcocastellaro)  converted from Enhanced DICOM to Classic DICOM
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -750,16 +750,16 @@
       </c>
       <c r="Z2" t="inlineStr">
         <is>
-          <t>[1306.3 1195.7 1258.8 1389.5 1484.2 1217.3 1236.7 1223.9 1314.8 1347.
- 1210.2 1220.4 1250.9 1177.3 1136.7 1212.8 1193.6 1268.3 1199.9 1099.1
- 1225.8 1282.4 1344.7 1279.1 1155.5]</t>
+          <t>[ 928.4  861.1  909.5  992.1 1049.1  869.6  882.5  878.7  939.1  966.
+  863.9  869.7  894.1  851.   831.8  866.9  855.1  901.8  858.8  800.3
+  871.8  909.8  943.   896.8  831.5]</t>
         </is>
       </c>
       <c r="AA2" t="inlineStr">
         <is>
-          <t>[1283.8 1308.3 1358.2 1352.2 1299.9 1303.  1264.4 1329.1 1357.4 1287.7
- 1349.8 1303.7 1313.8 1290.3 1272.2 1257.5 1252.7 1258.8 1202.8 1215.2
- 1303.2 1267.8 1224.4 1221.8 1228.2]</t>
+          <t>[912.6 925.7 953.9 950.5 922.4 926.4 904.  944.1 959.5 915.5 951.3 928.4
+ 935.7 920.5 907.  898.3 898.2 903.2 865.1 872.1 928.7 905.4 880.9 878.1
+ 878.3]</t>
         </is>
       </c>
       <c r="AB2" t="inlineStr">
@@ -769,9 +769,9 @@
       </c>
       <c r="AC2" t="inlineStr">
         <is>
-          <t>[4074.4 2741.4 2492.2 2785.8 2123.1 1952.  2478.3 2212.7 1949.5 2532.7
- 2518.8 2657.4 2587.  2568.3 2650.7 2704.4 2822.1 2775.  2592.4 2399.8
- 2368.2 2452.7 2320.4 2600.7 2505.6 2293.5 2668. ]</t>
+          <t>[2140.6 1676.3 1576.7 1700.7 1413.  1322.2 1579.2 1455.9 1321.4 1596.9
+ 1588.8 1648.5 1624.3 1619.  1657.2 1668.8 1723.5 1711.2 1603.7 1537.6
+ 1532.2 1542.5 1498.6 1624.7 1562.7 1476.6 1650.6]</t>
         </is>
       </c>
       <c r="AD2" t="inlineStr"/>
@@ -2573,30 +2573,30 @@
       </c>
       <c r="Z15" t="inlineStr">
         <is>
-          <t>[566.  580.9 552.  570.1 658.1 583.1 593.1 564.5 572.3 585.3 564.9 561.1
- 540.6 555.5 549.1 547.1 559.8 522.7 533.5 530.8 556.6 553.5 527.6 546.1
- 547.1]</t>
+          <t>[798.7 811.8 780.3 818.8 888.4 819.7 835.  792.  809.1 834.2 818.  802.5
+ 773.1 796.3 794.4 794.8 790.5 736.1 766.3 770.5 788.6 799.4 751.8 778.1
+ 798.9]</t>
         </is>
       </c>
       <c r="AA15" t="inlineStr">
         <is>
-          <t>[566.5 583.  573.9 569.1 578.9 565.  584.3 543.5 558.6 582.7 546.4 570.1
- 547.3 571.8 589.6 526.7 552.8 537.4 533.6 574.6 546.1 571.2 550.9 537.8
- 574.1]</t>
+          <t>[775.2 810.1 792.1 764.8 778.  789.9 802.6 753.3 767.4 801.7 758.1 794.
+ 772.9 798.6 818.6 733.5 759.2 753.1 738.9 777.8 779.5 792.7 773.2 740.3
+ 778.1]</t>
         </is>
       </c>
       <c r="AB15" t="inlineStr">
         <is>
-          <t>[ 977.2  968.6 1038.9 1032.2 1003.   974.4  986.7 1015.1  981.4  992.3
- 1005.2 1072.  1041.6 1001.7  982.6 1073.7 1053.8 1031.8 1050.5 1057.9
- 1133.1 1082.7 1043.4 1047.5 1084.6]</t>
+          <t>[1184.  1238.9 1309.2 1296.6 1241.8 1204.5 1220.  1267.1 1223.9 1236.8
+ 1231.7 1321.5 1292.  1226.8 1212.3 1313.5 1293.3 1258.7 1299.4 1311.5
+ 1417.9 1340.  1278.5 1307.9 1325.7]</t>
         </is>
       </c>
       <c r="AC15" t="inlineStr">
         <is>
-          <t>[1268.  1296.8 1284.2 1266.  1280.6 1303.5 1309.4 1257.6 1250.2 1270.
- 1154.8 1129.9 1293.4 1202.6 1128.  1305.3 1207.5 1178.7 1572.7 1463.8
- 1364.5 1665.5 1438.9 1359.4 1679.5 1397.5 1297.3]</t>
+          <t>[1559.1 1591.4 1567.1 1530.5 1574.6 1591.8 1624.8 1554.5 1515.6 1571.1
+ 1439.1 1410.2 1628.  1519.  1406.3 1667.7 1512.4 1482.1 2009.2 1822.5
+ 1677.  2217.  1771.8 1729.4 2199.9 1710.9 1623.9]</t>
         </is>
       </c>
       <c r="AD15" t="inlineStr"/>

</xml_diff>

<commit_message>
Fix labels in 20200207_jorgejovicich_cimec_human where deep GM was mislabeled as cortical GM
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -2165,17 +2165,16 @@
       </c>
       <c r="AB12" t="inlineStr">
         <is>
+          <t>[ 938.7  949.3  860.4  983.2 1024.5 1054.9 1033.   832.2 1013.6  964.
+ 1040.6 1041.5 1055.4 1144.5 1023.9 1055.  1000.1 1329.  1033.8  971.4
+ 1113.2 1109.8 1227.  1082.3  939.1]</t>
+        </is>
+      </c>
+      <c r="AC12" t="inlineStr">
+        <is>
           <t>[1520.5 1302.7 1250.1 1351.9 1387.7 1483.7 1241.3 1278.1 1254.  1573.5
- 1919.8 1512.1 1516.2 1357.7 1234.4 1307.6 1215.7 1207.8  938.7  949.3
-  860.4  983.2 1024.5 1054.9 1033.   832.2 1013.6  964.  1040.6 1041.5
- 1055.4 1144.5 1023.9 1055.  1000.1 1329.  1033.8  971.4 1113.2 1109.8
- 1227.  1082.3  939.1 1376.5 1294.3 1501.2 1411.4 1390.9 1449.6 1212.1
- 1110.9 1365.4]</t>
-        </is>
-      </c>
-      <c r="AC12" t="inlineStr">
-        <is>
-          <t>[]</t>
+ 1919.8 1512.1 1516.2 1357.7 1234.4 1307.6 1215.7 1207.8 1376.5 1294.3
+ 1501.2 1411.4 1390.9 1449.6 1212.1 1110.9 1365.4]</t>
         </is>
       </c>
       <c r="AD12" t="inlineStr"/>

</xml_diff>

<commit_message>
Update notebooks and database for fixed ROI
</commit_message>
<xml_diff>
--- a/databases/3T_human_T1maps_database.xlsx
+++ b/databases/3T_human_T1maps_database.xlsx
@@ -5239,9 +5239,9 @@
       </c>
       <c r="AA34" t="inlineStr">
         <is>
-          <t>[ 813.1  813.2  825.6  820.   864.1  847.   778.3  838.6  827.1  849.3
- 1093.5  810.8  825.2  855.4  864.8 1423.5  930.8  796.9  830.6  814.3
- 1454.5 1033.   809.   825.5  829.1]</t>
+          <t>[848.5 868.7 858.5 852.7 846.2 824.5 849.  878.1 894.3 873.8 835.9 794.7
+ 821.4 840.7 823.6 852.4 796.2 807.1 794.1 818.5 824.9 815.6 823.5 811.2
+ 872.5]</t>
         </is>
       </c>
       <c r="AB34" t="inlineStr">
@@ -5380,9 +5380,9 @@
       </c>
       <c r="AA35" t="inlineStr">
         <is>
-          <t>[ 814.5  820.5  838.1  830.4  852.2  849.4  782.4  844.4  835.5  845.7
- 1095.2  811.   832.9  851.1  854.8 1418.1  928.5  799.4  823.7  823.6
- 1454.1 1031.6  809.6  823.3  831.8]</t>
+          <t>[855.7 850.3 847.7 844.  808.9 855.6 862.7 872.3 860.3 829.9 823.7 829.9
+ 841.  831.4 818.5 816.3 821.8 813.2 829.5 826.8 831.1 833.4 824.7 861.8
+ 840.1]</t>
         </is>
       </c>
       <c r="AB35" t="inlineStr">

</xml_diff>